<commit_message>
FIX: When changing to quizzes at start up
</commit_message>
<xml_diff>
--- a/grading/all_form_responses.xlsx
+++ b/grading/all_form_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:U7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,47 +456,47 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>Overall grade to this team's Slide deck?</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Contribution of research to your skill/knowledge</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Your Full Name</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Have reviewed the paper?</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Paper manuscript format/organization</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Paper content material benefits you?</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Feedback to the team</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Overall grade to this team's Research topic and (summary) paper content?</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Email</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
@@ -539,49 +539,49 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ACYDBNiNcglCa_bKzlUfqFVyIZSEGubGxYsuDyp9br4yX2wIDv4jYDnkO11OLkPByjNekUg</t>
+          <t>ACYDBNgam9zyzlTamRzevyI2ASOQ1IQkKuwrFxfV35mu8h-njPRCehR0TcVo4mJVVtW3CbQ</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2024-12-05T21:48:43.825Z</t>
+          <t>2024-12-06T08:02:36.843Z</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2024-12-05T21:48:43.825499Z</t>
+          <t>2024-12-06T08:02:36.843004Z</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>Kevin.LopezChavez01@student.csulb.edu</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Satisfactory</t>
+          <t>6</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>kevin</t>
+          <t>Satisfactory</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
+          <t>Kevin</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Satisfactory</t>
-        </is>
-      </c>
       <c r="J2" t="inlineStr">
         <is>
           <t>Satisfactory</t>
@@ -589,17 +589,17 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
+          <t>Satisfactory</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
           <t>asdf</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>Kevin.LopezChavez01@student.csulb.edu</t>
+          <t>5</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
@@ -634,7 +634,7 @@
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>SampleTeam new</t>
+          <t>SampleTeam</t>
         </is>
       </c>
       <c r="U2" t="inlineStr"/>
@@ -642,105 +642,517 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>ACYDBNiNcglCa_bKzlUfqFVyIZSEGubGxYsuDyp9br4yX2wIDv4jYDnkO11OLkPByjNekUg</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2024-12-05T21:48:43.825Z</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2024-12-05T21:48:43.825499Z</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Kevin.LopezChavez01@student.csulb.edu</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Satisfactory</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>kevin</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Satisfactory</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Satisfactory</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Satisfactory</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>Satisfactory</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>Satisfactory</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>Satisfactory</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>SampleTeam3</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ACYDBNiNcglCa_bKzlUfqFVyIZSEGubGxYsuDyp9br4yX2wIDv4jYDnkO11OLkPByjNekUg</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2024-12-05T21:48:43.825Z</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2024-12-05T21:48:43.825499Z</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Kevin.LopezChavez01@student.csulb.edu</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Satisfactory</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>kevin</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Satisfactory</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Satisfactory</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>Satisfactory</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>Satisfactory</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>Satisfactory</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>Satisfactory</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>SampleTeam new</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
           <t>ACYDBNioo_Ef_xV6NEE3k36AadVfjFeQ8KH4KxcOoRzGrK86-J-2DR8AQ14OKjRTOG0cBIs</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>2024-12-05T22:35:47.281Z</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>2024-12-05T22:35:47.281785Z</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>8</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Kevin.LopezChavez01@student.csulb.edu</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
         <is>
           <t>8</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Satisfactory</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Satisfactory</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
         <is>
           <t>Kevin Lopez</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Satisfactory</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>Satisfactory</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Satisfactory</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Satisfactory</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
         <is>
           <t>asdf</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="M5" t="inlineStr">
         <is>
           <t>8</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>Satisfactory</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Satisfactory</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>Satisfactory</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>Satisfactory</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>SampleTeam new 2</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>ACYDBNhcQTziMqJg6x8y_NfBCG3rX7AAhWxabBVv5roIHJ8uHYXSg01Dotg5GOFwr76V9XE</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2024-12-06T02:39:18.354Z</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2024-12-06T02:39:18.354929Z</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>jerry.wu01@student.csulb.edu</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Satisfactory</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Jerry Wu</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Satisfactory</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Satisfactory</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>adfa</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>adfa</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>Satisfactory</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>Satisfactory</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>Satisfactory</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>Satisfactory</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>JErryS project</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>ACYDBNgfo1VX5jhx0rKKHP8wkot-gVKSki78Bt_6JH-noKm4-3AOPxRHXRcGKnMXeq27j14</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2024-12-06T02:39:09.537Z</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2024-12-06T02:39:09.537431Z</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
         <is>
           <t>Kevin.LopezChavez01@student.csulb.edu</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr">
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Satisfactory</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Kevin Lopez Chavez</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Satisfactory</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Satisfactory</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
         <is>
           <t>asdf</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>Satisfactory</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>Satisfactory</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>Satisfactory</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>Satisfactory</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>Satisfactory</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>Satisfactory</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>Satisfactory</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>SampleTeam new 2</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr"/>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>Satisfactory</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>JErryS project</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>